<commit_message>
popgen and figure updates
</commit_message>
<xml_diff>
--- a/Data/glct_causality/6-24-2019_glct-3_BRC20067_TGA.xlsx
+++ b/Data/glct_causality/6-24-2019_glct-3_BRC20067_TGA.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huiminna/Desktop/Erik_mapping/QTL paper/DATA/10-19-2015 12 strain PA curve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huiminna/Desktop/GWAS/QTL paper/DATA/10-19-2015 12 strain PA curve/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="6-24-2019" sheetId="1" r:id="rId1"/>
     <sheet name="6-28-2019" sheetId="2" r:id="rId2"/>
+    <sheet name="9-1-2019" sheetId="4" r:id="rId3"/>
+    <sheet name="9-9-2019" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
   <si>
     <t>BRC20067</t>
   </si>
@@ -64,6 +66,39 @@
   </si>
   <si>
     <t>Replicate3</t>
+  </si>
+  <si>
+    <t>Replicate-1</t>
+  </si>
+  <si>
+    <t>Replicate-2</t>
+  </si>
+  <si>
+    <t>Replicate-3</t>
+  </si>
+  <si>
+    <t>Replicate-4</t>
+  </si>
+  <si>
+    <t>Replicate-5</t>
+  </si>
+  <si>
+    <t>Replicate-6</t>
+  </si>
+  <si>
+    <t>day0</t>
+  </si>
+  <si>
+    <t>day2</t>
+  </si>
+  <si>
+    <t>day2/day0</t>
+  </si>
+  <si>
+    <t>glct-3_57nt</t>
+  </si>
+  <si>
+    <t>glct-3_TGA</t>
   </si>
 </sst>
 </file>
@@ -129,7 +164,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -137,6 +172,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -506,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -720,4 +758,982 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K19:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>136</v>
+      </c>
+      <c r="C3" s="1">
+        <v>122</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3/B3*100</f>
+        <v>89.705882352941174</v>
+      </c>
+      <c r="E3" s="1">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3/E3*100</f>
+        <v>87.671232876712324</v>
+      </c>
+      <c r="H3" s="1">
+        <v>83</v>
+      </c>
+      <c r="I3" s="1">
+        <v>68</v>
+      </c>
+      <c r="J3" s="1">
+        <f>I3/H3*100</f>
+        <v>81.92771084337349</v>
+      </c>
+      <c r="K3" s="1">
+        <v>55</v>
+      </c>
+      <c r="L3" s="1">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1">
+        <f>L3/K3*100</f>
+        <v>80</v>
+      </c>
+      <c r="N3" s="1">
+        <v>35</v>
+      </c>
+      <c r="O3" s="1">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1">
+        <f>O3/N3*100</f>
+        <v>88.571428571428569</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>78</v>
+      </c>
+      <c r="R3" s="1">
+        <v>70</v>
+      </c>
+      <c r="S3" s="1">
+        <f>R3/Q3*100</f>
+        <v>89.743589743589752</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D6" si="0">C4/B4*100</f>
+        <v>43.75</v>
+      </c>
+      <c r="E4" s="1">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G6" si="1">F4/E4*100</f>
+        <v>57.407407407407405</v>
+      </c>
+      <c r="H4" s="1">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J6" si="2">I4/H4*100</f>
+        <v>42.424242424242422</v>
+      </c>
+      <c r="K4" s="1">
+        <v>58</v>
+      </c>
+      <c r="L4" s="1">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M6" si="3">L4/K4*100</f>
+        <v>34.482758620689658</v>
+      </c>
+      <c r="N4" s="1">
+        <v>40</v>
+      </c>
+      <c r="O4" s="1">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P6" si="4">O4/N4*100</f>
+        <v>32.5</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>54</v>
+      </c>
+      <c r="R4" s="1">
+        <v>34</v>
+      </c>
+      <c r="S4" s="1">
+        <f t="shared" ref="S4:S6" si="5">R4/Q4*100</f>
+        <v>62.962962962962962</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="E5" s="1">
+        <v>87</v>
+      </c>
+      <c r="F5" s="1">
+        <v>62</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>71.264367816091962</v>
+      </c>
+      <c r="H5" s="1">
+        <v>87</v>
+      </c>
+      <c r="I5" s="1">
+        <v>59</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>67.81609195402298</v>
+      </c>
+      <c r="K5" s="1">
+        <v>110</v>
+      </c>
+      <c r="L5" s="1">
+        <v>40</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="3"/>
+        <v>36.363636363636367</v>
+      </c>
+      <c r="N5" s="1">
+        <v>48</v>
+      </c>
+      <c r="O5" s="1">
+        <v>26</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="4"/>
+        <v>54.166666666666664</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>101</v>
+      </c>
+      <c r="R5" s="1">
+        <v>71</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" si="5"/>
+        <v>70.297029702970292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>57.777777777777771</v>
+      </c>
+      <c r="E6" s="1">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>68.571428571428569</v>
+      </c>
+      <c r="H6" s="1">
+        <v>51</v>
+      </c>
+      <c r="I6" s="1">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>56.862745098039213</v>
+      </c>
+      <c r="K6" s="1">
+        <v>123</v>
+      </c>
+      <c r="L6" s="1">
+        <v>101</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="3"/>
+        <v>82.113821138211378</v>
+      </c>
+      <c r="N6" s="1">
+        <v>50</v>
+      </c>
+      <c r="O6" s="1">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>58</v>
+      </c>
+      <c r="R6" s="1">
+        <v>48</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="5"/>
+        <v>82.758620689655174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>89.705882352941174</v>
+      </c>
+      <c r="C10" s="1">
+        <v>87.671232876712324</v>
+      </c>
+      <c r="D10" s="1">
+        <v>81.92771084337349</v>
+      </c>
+      <c r="E10" s="1">
+        <v>80</v>
+      </c>
+      <c r="F10" s="1">
+        <v>88.571428571428569</v>
+      </c>
+      <c r="G10" s="1">
+        <v>89.743589743589752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43.75</v>
+      </c>
+      <c r="C11" s="1">
+        <v>57.407407407407405</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42.424242424242422</v>
+      </c>
+      <c r="E11" s="1">
+        <v>34.482758620689658</v>
+      </c>
+      <c r="F11" s="1">
+        <v>32.5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>62.962962962962962</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>66.666666666666657</v>
+      </c>
+      <c r="C12" s="1">
+        <v>71.264367816091962</v>
+      </c>
+      <c r="D12" s="1">
+        <v>67.81609195402298</v>
+      </c>
+      <c r="E12" s="1">
+        <v>36.363636363636367</v>
+      </c>
+      <c r="F12" s="1">
+        <v>54.166666666666664</v>
+      </c>
+      <c r="G12" s="1">
+        <v>70.297029702970292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>57.777777777777771</v>
+      </c>
+      <c r="C13" s="1">
+        <v>68.571428571428569</v>
+      </c>
+      <c r="D13" s="1">
+        <v>56.862745098039213</v>
+      </c>
+      <c r="E13" s="1">
+        <v>82.113821138211378</v>
+      </c>
+      <c r="F13" s="1">
+        <v>82</v>
+      </c>
+      <c r="G13" s="1">
+        <v>82.758620689655174</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3/B3*100</f>
+        <v>77.777777777777786</v>
+      </c>
+      <c r="E3" s="1">
+        <v>69</v>
+      </c>
+      <c r="F3" s="1">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3/E3*100</f>
+        <v>75.362318840579718</v>
+      </c>
+      <c r="H3" s="1">
+        <v>64</v>
+      </c>
+      <c r="I3" s="1">
+        <v>51</v>
+      </c>
+      <c r="J3" s="1">
+        <f>I3/H3*100</f>
+        <v>79.6875</v>
+      </c>
+      <c r="K3" s="1">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1">
+        <f>L3/K3*100</f>
+        <v>87.5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>81</v>
+      </c>
+      <c r="O3" s="1">
+        <v>67</v>
+      </c>
+      <c r="P3" s="1">
+        <f>O3/N3*100</f>
+        <v>82.716049382716051</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>44</v>
+      </c>
+      <c r="R3" s="1">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1">
+        <f>R3/Q3*100</f>
+        <v>81.818181818181827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D6" si="0">C4/B4*100</f>
+        <v>28.125</v>
+      </c>
+      <c r="E4" s="1">
+        <v>76</v>
+      </c>
+      <c r="F4" s="1">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G6" si="1">F4/E4*100</f>
+        <v>23.684210526315788</v>
+      </c>
+      <c r="H4" s="1">
+        <v>90</v>
+      </c>
+      <c r="I4" s="1">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J6" si="2">I4/H4*100</f>
+        <v>17.777777777777779</v>
+      </c>
+      <c r="K4" s="1">
+        <v>88</v>
+      </c>
+      <c r="L4" s="1">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M6" si="3">L4/K4*100</f>
+        <v>23.863636363636363</v>
+      </c>
+      <c r="N4" s="1">
+        <v>54</v>
+      </c>
+      <c r="O4" s="1">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P6" si="4">O4/N4*100</f>
+        <v>24.074074074074073</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>58</v>
+      </c>
+      <c r="R4" s="1">
+        <v>3</v>
+      </c>
+      <c r="S4" s="1">
+        <f t="shared" ref="S4:S6" si="5">R4/Q4*100</f>
+        <v>5.1724137931034484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>102</v>
+      </c>
+      <c r="C5" s="1">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>25.490196078431371</v>
+      </c>
+      <c r="E5" s="1">
+        <v>108</v>
+      </c>
+      <c r="F5" s="1">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>14.814814814814813</v>
+      </c>
+      <c r="H5" s="1">
+        <v>53</v>
+      </c>
+      <c r="I5" s="1">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>24.528301886792452</v>
+      </c>
+      <c r="K5" s="1">
+        <v>48</v>
+      </c>
+      <c r="L5" s="1">
+        <v>28</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="3"/>
+        <v>58.333333333333336</v>
+      </c>
+      <c r="N5" s="1">
+        <v>66</v>
+      </c>
+      <c r="O5" s="1">
+        <v>26</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="4"/>
+        <v>39.393939393939391</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>101</v>
+      </c>
+      <c r="R5" s="1">
+        <v>22</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" si="5"/>
+        <v>21.782178217821784</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>51.020408163265309</v>
+      </c>
+      <c r="E6" s="1">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>67.796610169491515</v>
+      </c>
+      <c r="H6" s="1">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="K6" s="1">
+        <v>64</v>
+      </c>
+      <c r="L6" s="1">
+        <v>46</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="3"/>
+        <v>71.875</v>
+      </c>
+      <c r="N6" s="1">
+        <v>52</v>
+      </c>
+      <c r="O6" s="1">
+        <v>25</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="4"/>
+        <v>48.07692307692308</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>43</v>
+      </c>
+      <c r="R6" s="1">
+        <v>18</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="5"/>
+        <v>41.860465116279073</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>77.777777777777786</v>
+      </c>
+      <c r="C12" s="1">
+        <v>75.362318840579718</v>
+      </c>
+      <c r="D12" s="1">
+        <v>79.6875</v>
+      </c>
+      <c r="E12" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>82.716049382716051</v>
+      </c>
+      <c r="G12" s="1">
+        <v>81.818181818181827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28.125</v>
+      </c>
+      <c r="C13" s="1">
+        <v>23.684210526315788</v>
+      </c>
+      <c r="D13" s="1">
+        <v>17.777777777777779</v>
+      </c>
+      <c r="E13" s="1">
+        <v>23.863636363636363</v>
+      </c>
+      <c r="F13" s="1">
+        <v>24.074074074074073</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.1724137931034484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>25.490196078431371</v>
+      </c>
+      <c r="C14" s="1">
+        <v>14.814814814814813</v>
+      </c>
+      <c r="D14" s="1">
+        <v>24.528301886792452</v>
+      </c>
+      <c r="E14" s="1">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="F14" s="1">
+        <v>39.393939393939391</v>
+      </c>
+      <c r="G14" s="1">
+        <v>21.782178217821784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
+        <v>51.020408163265309</v>
+      </c>
+      <c r="C15" s="1">
+        <v>67.796610169491515</v>
+      </c>
+      <c r="D15" s="1">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1">
+        <v>71.875</v>
+      </c>
+      <c r="F15" s="1">
+        <v>48.07692307692308</v>
+      </c>
+      <c r="G15" s="1">
+        <v>41.860465116279073</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>